<commit_message>
Working on report  View
</commit_message>
<xml_diff>
--- a/HopeAcademySMS/Content/ExcelUploadedFile/ResultTest.xlsx
+++ b/HopeAcademySMS/Content/ExcelUploadedFile/ResultTest.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$17</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="29">
   <si>
     <t>StudentNumber</t>
   </si>
@@ -50,15 +53,6 @@
     <t>Teachername</t>
   </si>
   <si>
-    <t>SS-2A-014</t>
-  </si>
-  <si>
-    <t>SS-2A-015</t>
-  </si>
-  <si>
-    <t>STA</t>
-  </si>
-  <si>
     <t>GT</t>
   </si>
   <si>
@@ -66,14 +60,76 @@
   </si>
   <si>
     <t>First</t>
+  </si>
+  <si>
+    <t>HAS-015-013</t>
+  </si>
+  <si>
+    <t>HAS-015-014</t>
+  </si>
+  <si>
+    <t>HAS-015-015</t>
+  </si>
+  <si>
+    <t>HAS-015-016</t>
+  </si>
+  <si>
+    <t>HAS-015-017</t>
+  </si>
+  <si>
+    <t>HAS-015-018</t>
+  </si>
+  <si>
+    <t>HAS-015-019</t>
+  </si>
+  <si>
+    <t>HAS-015-020</t>
+  </si>
+  <si>
+    <t>HAS-015-021</t>
+  </si>
+  <si>
+    <t>HAS-015-022</t>
+  </si>
+  <si>
+    <t>HAS-015-023</t>
+  </si>
+  <si>
+    <t>HAS-015-024</t>
+  </si>
+  <si>
+    <t>HAS-015-025</t>
+  </si>
+  <si>
+    <t>HAS-015-026</t>
+  </si>
+  <si>
+    <t>HAS-015-027</t>
+  </si>
+  <si>
+    <t>HAS-015-028</t>
+  </si>
+  <si>
+    <t>Sessoion</t>
+  </si>
+  <si>
+    <t>2016-2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -89,10 +145,64 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -101,13 +211,212 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -417,14 +726,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I5"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="6" max="7" width="14" customWidth="1"/>
@@ -432,137 +742,602 @@
     <col min="9" max="9" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1">
+        <v>32.5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>19</v>
+      </c>
+      <c r="F11" s="1">
+        <v>27.5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F14" s="1">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D15" s="3">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3">
+        <v>7</v>
+      </c>
+      <c r="F15" s="3">
+        <v>38</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4">
+        <v>19</v>
+      </c>
+      <c r="F16" s="4">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="5">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>8</v>
-      </c>
-      <c r="F2">
+      <c r="D17" s="5">
         <v>5</v>
       </c>
-      <c r="G2">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="E17" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>20</v>
-      </c>
-      <c r="G5">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
+      <c r="F17" s="5">
+        <v>28</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D17"/>
+  <conditionalFormatting sqref="F2:F17">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="lessThan">
+      <formula>20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="lessThan">
+      <formula>20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="lessThan">
+      <formula>20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThan">
+      <formula>20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="lessThan">
+      <formula>20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E17">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="lessThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C17">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D17">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>